<commit_message>
Moved session creation out of do_set_ign. Added GO Rating to set_ign message. Added get_official_rating Added test_get_official_rating
</commit_message>
<xml_diff>
--- a/go_post_s10_adjusted_ratings.xlsx
+++ b/go_post_s10_adjusted_ratings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stube/Documents/developer/GoBot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21CA5247-F855-1D47-9677-809C38726C2B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E999BEB-C6EE-014C-B9F7-D4FA56A8D7D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="31840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="477" uniqueCount="247">
   <si>
     <t>ign</t>
   </si>
@@ -776,6 +776,9 @@
   </si>
   <si>
     <t>Z_90</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1735,7 +1738,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AA4E7F1-9005-694F-9017-06451A505FAF}">
-  <dimension ref="A1:P222"/>
+  <dimension ref="A1:T222"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="125" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -2470,7 +2473,7 @@
         <v>1.6451931974644256</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
         <v>214</v>
       </c>
@@ -2514,7 +2517,7 @@
         <v>1.5421944747482916</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
         <v>90</v>
       </c>
@@ -2558,7 +2561,7 @@
         <v>1.5091334814500359</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>79</v>
       </c>
@@ -2602,7 +2605,7 @@
         <v>1.4938320601115691</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="7" t="s">
         <v>143</v>
       </c>
@@ -2646,7 +2649,7 @@
         <v>1.486483172703071</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A21" s="7" t="s">
         <v>213</v>
       </c>
@@ -2690,7 +2693,7 @@
         <v>1.3953104834346628</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A22" s="7" t="s">
         <v>180</v>
       </c>
@@ -2734,7 +2737,7 @@
         <v>1.3778927238227572</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>31</v>
       </c>
@@ -2778,7 +2781,7 @@
         <v>1.3431348777366625</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>179</v>
       </c>
@@ -2822,7 +2825,7 @@
         <v>1.3402366191242443</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A25" s="7" t="s">
         <v>155</v>
       </c>
@@ -2866,7 +2869,7 @@
         <v>1.3113436347656964</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A26" s="7" t="s">
         <v>196</v>
       </c>
@@ -2910,7 +2913,7 @@
         <v>1.289621947542533</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A27" s="7" t="s">
         <v>32</v>
       </c>
@@ -2954,7 +2957,7 @@
         <v>1.2564876443389041</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="7" t="s">
         <v>198</v>
       </c>
@@ -2997,8 +3000,11 @@
         <f>(H28-$O$2)/$O$3</f>
         <v>1.2557911613179</v>
       </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="T28" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A29" s="7" t="s">
         <v>217</v>
       </c>
@@ -3042,7 +3048,7 @@
         <v>1.2440421361933982</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A30" s="7" t="s">
         <v>146</v>
       </c>
@@ -3086,7 +3092,7 @@
         <v>1.150443855172433</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A31" s="7" t="s">
         <v>192</v>
       </c>
@@ -3130,7 +3136,7 @@
         <v>1.0622724976281408</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="7" t="s">
         <v>229</v>
       </c>

</xml_diff>